<commit_message>
Added new tree problems
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265504CD-1882-9445-BBC3-8ABD734EC0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B83410-CFCC-174F-B3A3-090C40C394C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4660" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Problem</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Solution</t>
+  </si>
+  <si>
+    <t>Maximun Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-depth-of-binary-tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use recursive DFS approach to count depth. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use recursive DFS approach to check values of nodes. </t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Return binary tree's maximum depth.</t>
+  </si>
+  <si>
+    <t>Check if binary trees are same.</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Invert given binary tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use recursive DFS to invert subtrees </t>
+  </si>
+  <si>
+    <t>Subtree of Another Tree</t>
+  </si>
+  <si>
+    <t>Check if tree is subtree of another tree.</t>
+  </si>
+  <si>
+    <t>Use recursive DFS to traverse thru nodes and call isSameTree function to check weather trees are same.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/subtree-of-another-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/invert-binary-tree/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -57,20 +111,72 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="20"/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -82,16 +188,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,27 +522,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="187.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="58" style="1" customWidth="1"/>
+    <col min="3" max="3" width="187.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{81FA332A-8EF1-4549-A3E8-9DC47654C3CA}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{75605A2A-2A43-D74F-99C7-EE6AE9B1387A}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{DB61C639-19F1-AB43-B8C0-AC6D20C4E12B}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{AE1502FC-4861-0F43-8DE9-AF0402F1CF4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new graph problems
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F4DD45-379A-3C43-AF13-1B4E2494C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9CF33-A2DF-D84C-9025-4DD9B9CCFDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="4500" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Solution</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>Use stack to iteratively DFS Inorder traverse on a tree. If prevous value is greater than current, return false;</t>
+  </si>
+  <si>
+    <t>Graph Valid Tree</t>
+  </si>
+  <si>
+    <t>Return true if provided graph is a tree</t>
+  </si>
+  <si>
+    <t>Create adjacency List of list. Use stack to iteratively DFS traverse. Keep track of visited neighbors using a set. Keep remove backpointer from the adjacency list. If numNodes == set size, return true. If current node already in the set, return false</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/validate-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/graph-valid-tree/</t>
   </si>
 </sst>
 </file>
@@ -577,17 +595,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="48.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="197" style="1" customWidth="1"/>
+    <col min="3" max="3" width="197.1640625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -699,6 +717,9 @@
       <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -709,6 +730,23 @@
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -719,6 +757,9 @@
     <hyperlink ref="D4" r:id="rId4" xr:uid="{AE1502FC-4861-0F43-8DE9-AF0402F1CF4D}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{7B6AA6D1-BC4B-2F4B-B8CC-B2273F527AED}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{A85D9E62-8269-804F-80E7-53A9EB46BCB6}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{187E11BF-B774-154E-B958-04088916D203}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{3134FC51-1C7C-6A41-94C1-26AA43037DF5}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{3E1F2737-CB99-404C-A64B-A178B257FADC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Array problems
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B9CF33-A2DF-D84C-9025-4DD9B9CCFDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B43F638-0980-144C-A9B3-D6A1CA37CCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Solution</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/graph-valid-tree/</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self</t>
+  </si>
+  <si>
+    <t>Return array of product of each element except current</t>
+  </si>
+  <si>
+    <t>Create prefix and postfix product array. Calculate prefix and postfix products and return array by multiplying both</t>
   </si>
 </sst>
 </file>
@@ -595,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -747,6 +756,17 @@
       </c>
       <c r="D10" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new DP problems
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C82CFE4-DCB7-B64D-BD52-AD33291A1B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F53276-BA2B-614F-88A9-5B9FDFB57EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17220" yWindow="760" windowWidth="17340" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Solution</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>Use a bottom-up approach using for loop and an array. Subproblem: dp[n] = dp[n-1] + dp[n-2]</t>
+  </si>
+  <si>
+    <t>House Robber</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/house-robber/</t>
+  </si>
+  <si>
+    <t>Return maximum ammount without robbing adjacent houses</t>
+  </si>
+  <si>
+    <t>Use a bottom-up approach using for loop and an array. Subproblem: dp[n] = Math.max(dp[n-1], dp[n-2] + nums[n])</t>
   </si>
 </sst>
 </file>
@@ -685,9 +697,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -949,6 +961,20 @@
       </c>
       <c r="D18" s="3" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -970,6 +996,7 @@
     <hyperlink ref="D16" r:id="rId15" xr:uid="{CE5AA9F6-D3B2-444D-90F6-C463623EC47C}"/>
     <hyperlink ref="D17" r:id="rId16" xr:uid="{676BCF16-5E47-7F43-B129-6C0ECAB8A1FD}"/>
     <hyperlink ref="D18" r:id="rId17" xr:uid="{8BB9FA7E-5074-884F-BF96-701AE7B0C209}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{D2A0C53C-9515-D04F-8A69-1FEAB98A084E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new Matrix problem
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59339630-904F-B144-BAD5-328AEC13BA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3503E-E733-7145-9CCF-DEB9F406FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>Solution</t>
   </si>
@@ -267,6 +267,18 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/house-robber-ii/</t>
+  </si>
+  <si>
+    <t>Number of Islands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return num of islands made from adjacent '1' </t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-islands/</t>
+  </si>
+  <si>
+    <t>Iterate over grid using 2 for loops. If current is '1' increase numOfIslands, call recursive DFS function to mark all as visited(change it to '0')</t>
   </si>
 </sst>
 </file>
@@ -706,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -998,6 +1010,20 @@
       </c>
       <c r="D20" s="3" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1021,6 +1047,7 @@
     <hyperlink ref="D18" r:id="rId17" xr:uid="{8BB9FA7E-5074-884F-BF96-701AE7B0C209}"/>
     <hyperlink ref="D19" r:id="rId18" xr:uid="{D2A0C53C-9515-D04F-8A69-1FEAB98A084E}"/>
     <hyperlink ref="D20" r:id="rId19" xr:uid="{EC78446D-D8C2-7D41-A868-52C097CD1104}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{479A7FA6-FA6F-144D-B251-478FF39988F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new DP problem
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3503E-E733-7145-9CCF-DEB9F406FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F70749-F8DA-494B-AEA6-2937EE94FDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Solution</t>
   </si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>Iterate over grid using 2 for loops. If current is '1' increase numOfIslands, call recursive DFS function to mark all as visited(change it to '0')</t>
+  </si>
+  <si>
+    <t>Longest Common Subsequence</t>
+  </si>
+  <si>
+    <t>Return length of longest common subsequence</t>
+  </si>
+  <si>
+    <t>Use 2D DP array size of input length + 1 for base case 0. Iterate over strings comparing characters. If char is same, increase by one to the i-1,j-1 value.Else pick max from left and up value.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-common-subsequence/</t>
   </si>
 </sst>
 </file>
@@ -718,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1024,6 +1036,20 @@
       </c>
       <c r="D21" s="3" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1048,6 +1074,7 @@
     <hyperlink ref="D19" r:id="rId18" xr:uid="{D2A0C53C-9515-D04F-8A69-1FEAB98A084E}"/>
     <hyperlink ref="D20" r:id="rId19" xr:uid="{EC78446D-D8C2-7D41-A868-52C097CD1104}"/>
     <hyperlink ref="D21" r:id="rId20" xr:uid="{479A7FA6-FA6F-144D-B251-478FF39988F3}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{6CB87E9C-0C57-7A4B-B3F8-29E4D2759EFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new problems and cleaned code
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70AC365-EAF8-D84A-B5BC-B62CB713CE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B54BDBC-3962-414D-B62D-AD22B9DF16EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18300" yWindow="760" windowWidth="16260" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="109">
   <si>
     <t>Solution</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t xml:space="preserve">Sort each word from input array and create a map of sorted string and the list of original strings. Take values from Map and return as an ArrayList </t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>Return K top frequent elements</t>
+  </si>
+  <si>
+    <t>Use Map to map elements with their freqencies. Use priority queue to sort elements by its frequencies desc. Remove from pq and return as an array.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/top-k-frequent-elements/</t>
   </si>
 </sst>
 </file>
@@ -790,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1180,6 +1192,20 @@
       </c>
       <c r="D27" s="3" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1210,6 +1236,7 @@
     <hyperlink ref="D25" r:id="rId24" xr:uid="{AC58C7F5-E104-7A48-886C-8C26A9CADBDF}"/>
     <hyperlink ref="D26" r:id="rId25" xr:uid="{9D679823-129A-4148-A25B-7BF002095F37}"/>
     <hyperlink ref="D27" r:id="rId26" xr:uid="{BA9F6EFD-64FA-CB4D-9B45-3A55A614489B}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{226288BA-73B4-194E-9BB1-05A9F762705E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new problem structure
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPreps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202E9869-FB34-FF45-9315-CFD56C7D2756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88616C45-8497-9549-8D5B-1E808D4CBE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15280" yWindow="760" windowWidth="19280" windowHeight="19840" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19860" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="171">
   <si>
     <t>Solution</t>
   </si>
@@ -543,6 +543,12 @@
   </si>
   <si>
     <t>Use stack to maintain indices of the temperatures that are waiting for a warmer day. Iterate over temp array and add indeces of temp to stack while they are colder than curr temp. If warmer day found, update the waiting days using index from stack.</t>
+  </si>
+  <si>
+    <t>Car Fleet</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/car-fleet/</t>
   </si>
 </sst>
 </file>
@@ -983,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1600,10 +1606,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="1">
-        <f ca="1">C50</f>
-        <v>0</v>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1650,6 +1658,7 @@
     <hyperlink ref="D41" r:id="rId40" xr:uid="{AA85D42F-BC4F-8146-81DB-03775B9CB360}"/>
     <hyperlink ref="D42" r:id="rId41" xr:uid="{B8F5A6E1-8C02-9D46-8B76-37A0B34E9C8A}"/>
     <hyperlink ref="D43" r:id="rId42" xr:uid="{7A9E911C-89BC-3B48-9E80-AE85FAAEA921}"/>
+    <hyperlink ref="D44" r:id="rId43" xr:uid="{FE0D87B9-902B-0A43-8B5C-F222B9FA1123}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Union Find and Junit test
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPrep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7C47A3-3FC3-6F4B-8744-978377E4616C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA149A47-5D76-5B48-BE86-F8CCBEFB30E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>https://leetcode.com/problems/maximum-depth-of-binary-tree</t>
   </si>
   <si>
-    <t xml:space="preserve">Use recursive DFS approach to count depth. </t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Invert given binary tree</t>
   </si>
   <si>
-    <t xml:space="preserve">Use recursive DFS to invert subtrees </t>
-  </si>
-  <si>
     <t>Subtree of Another Tree</t>
   </si>
   <si>
@@ -816,6 +810,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/search-in-rotated-sorted-array/</t>
+  </si>
+  <si>
+    <t>Use recursive DFS to invert subtrees. Use temp to swap left and right child.</t>
+  </si>
+  <si>
+    <t>Use recursive DFS approach to count depth. Use variable to hold left and right length and return max length + 1(root).</t>
   </si>
 </sst>
 </file>
@@ -1258,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1273,10 +1273,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1287,16 +1287,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>258</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,10 +1304,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>259</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -1315,30 +1315,30 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,10 +1346,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -1357,839 +1357,839 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>257</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code and notes improvements
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renish/IdeaProjects/InterviewPrep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463D15A-7153-D945-B1D5-8105A95A0704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DF50BF-2A68-C14D-9086-D621624B0D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
+    <workbookView xWindow="19920" yWindow="760" windowWidth="14640" windowHeight="19880" xr2:uid="{08AB6A11-DBB1-E340-ABF9-8FDF47FDF74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="300">
   <si>
     <t>Solution</t>
   </si>
@@ -221,9 +221,6 @@
     <t>https://leetcode.com/problems/climbing-stairs/</t>
   </si>
   <si>
-    <t>Return dinstics way to climb for given steps</t>
-  </si>
-  <si>
     <t>Use a bottom-up approach using for loop and an array. Subproblem: dp[n] = dp[n-1] + dp[n-2]</t>
   </si>
   <si>
@@ -852,6 +849,93 @@
   </si>
   <si>
     <t xml:space="preserve">Create a TrieNode class which has an Array of TrieNode children and word end indicator. To implement 'insert' method, create a temp node to iterate over word tree. Iterate over word char by char and check if curr char is in the tree, if not, create a child node at the index. Keep iterating over word and create nodes and set end word indicator to true. For 'search' method, iterate same way over search word and return true if there is an end word indicator. </t>
+  </si>
+  <si>
+    <t>Use modified binary search. Check for two main conditions: subarray on left is sorted(i.e. nums[mid] &gt;= nums[left]) or right is sorted. If left is sorted and nums[left] &lt;= target &amp;&amp; target &lt; nums[mid], which means target is in left half else check right half.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/contains-duplicate/</t>
+  </si>
+  <si>
+    <t>Return true if given array contains duplicate number</t>
+  </si>
+  <si>
+    <t>Use hash set and iterate over array while adding items to the set. Return true if set.add doesn’t return false.</t>
+  </si>
+  <si>
+    <t>Contains Duplicate</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>Return true if given string is a palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/</t>
+  </si>
+  <si>
+    <t>Clean input by removing non-alphanum and converting it to lower case. Use two pointers to compare values at left and right pointers and return true if they all match.</t>
+  </si>
+  <si>
+    <t>Return distinct way to climb for given steps</t>
+  </si>
+  <si>
+    <t>Decode String</t>
+  </si>
+  <si>
+    <t>Return decoded string</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/decode-string/</t>
+  </si>
+  <si>
+    <t>Use two stacks to keep track of number in string and letters. Iterate over the string and if it's digits, push it onto the count stack. If '[' detected, push decorded string so far onto the string stack and reset decoded string. If ']' pop the last decoded string and build string.</t>
+  </si>
+  <si>
+    <t>Remove Duplicates from Sorted List</t>
+  </si>
+  <si>
+    <t>Return head of the sorted linked list</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/remove-duplicates-from-sorted-list/</t>
+  </si>
+  <si>
+    <t>Iterate over linked list while comparing curr.val to curr.next.val. If they're same curr.next = curr.next.next</t>
+  </si>
+  <si>
+    <t>Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>Return true if linked list is a palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-linked-list/</t>
+  </si>
+  <si>
+    <t>Use fast and slow pointers to find the median of the LL. Reverse second half of the LL. Compare first and second half and return false if their values does not match.</t>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
+  </si>
+  <si>
+    <t>Return reversed 32-bit integer</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/reverse-integer/</t>
+  </si>
+  <si>
+    <t>Keep num%10 to extract digits. To add to the result, result * 10 + digit. To check overflow, make sure (newResult - digit) / 10 != result. Remove last digit from the num by num/10.</t>
+  </si>
+  <si>
+    <t>Longest Absolute File Path</t>
+  </si>
+  <si>
+    <t>Return length of the max absolute path</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-absolute-file-path/</t>
   </si>
 </sst>
 </file>
@@ -1292,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F82D20-21B0-354D-9411-D7EE78EC7053}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1323,1023 +1407,1127 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>275</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>273</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>259</v>
+        <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>218</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>220</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>221</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>219</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>222</v>
+      <c r="A5" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>223</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>224</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>225</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>3</v>
+      <c r="A6" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>226</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
+      <c r="A7" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>227</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>102</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>237</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>236</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>228</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
+      <c r="A11" s="5" t="s">
+        <v>276</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>277</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>230</v>
+      <c r="A12" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>233</v>
+        <v>49</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>232</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>238</v>
+        <v>53</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>239</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>240</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>241</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>242</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>247</v>
+      <c r="A15" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>249</v>
+        <v>114</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>250</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>248</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>243</v>
+      <c r="A16" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>246</v>
+        <v>120</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>245</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>123</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>127</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>36</v>
+      <c r="A19" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>44</v>
+      <c r="A20" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>47</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>48</v>
+      <c r="A21" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>51</v>
+      <c r="A22" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>148</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>59</v>
+      <c r="A24" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>151</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>63</v>
+        <v>153</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>110</v>
+      <c r="A28" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>78</v>
+      <c r="A29" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>251</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>80</v>
+        <v>253</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>81</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>89</v>
+        <v>169</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>90</v>
+      <c r="A32" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>93</v>
+        <v>254</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>97</v>
+        <v>271</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>96</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>98</v>
+        <v>177</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>102</v>
+      <c r="A35" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>104</v>
+        <v>184</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>106</v>
+      <c r="A36" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>203</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>109</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>114</v>
+      <c r="A37" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>115</v>
+        <v>286</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>288</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>116</v>
+        <v>287</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>118</v>
+      <c r="A38" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>119</v>
+        <v>189</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>121</v>
+        <v>191</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>120</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>122</v>
+      <c r="A39" s="5" t="s">
+        <v>289</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>123</v>
+        <v>290</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>124</v>
+        <v>292</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>125</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>126</v>
+        <v>192</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>127</v>
+        <v>193</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>128</v>
+        <v>195</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>129</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>136</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>138</v>
+      <c r="A42" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>139</v>
+        <v>201</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>142</v>
+      <c r="A43" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>143</v>
+        <v>206</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>144</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>130</v>
+      <c r="A44" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>131</v>
+        <v>211</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>133</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>149</v>
+        <v>215</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>150</v>
+      <c r="A46" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>153</v>
+        <v>257</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>151</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>154</v>
+      <c r="A47" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>157</v>
+        <v>258</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>158</v>
+      <c r="A48" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>160</v>
+        <v>219</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>161</v>
+        <v>220</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>159</v>
+        <v>218</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>162</v>
+      <c r="A49" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>174</v>
+      <c r="A50" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>175</v>
+        <v>9</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>177</v>
+        <v>225</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>176</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>251</v>
+        <v>12</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>252</v>
+        <v>13</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>253</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>164</v>
+        <v>233</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>166</v>
+        <v>234</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>165</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>167</v>
+        <v>25</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>40</v>
+        <v>238</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>41</v>
+        <v>239</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>43</v>
+        <v>240</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>42</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>255</v>
+        <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>256</v>
+        <v>19</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>257</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>178</v>
+        <v>18</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>179</v>
+        <v>20</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>181</v>
+        <v>21</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>180</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>182</v>
+      <c r="A57" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>183</v>
+        <v>24</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>185</v>
+        <v>228</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>184</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>186</v>
+      <c r="A58" s="4" t="s">
+        <v>229</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>189</v>
+        <v>246</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>190</v>
+        <v>248</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>192</v>
+        <v>249</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>191</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>193</v>
+      <c r="A60" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>194</v>
+        <v>243</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>196</v>
+        <v>245</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>197</v>
+        <v>267</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>198</v>
+        <v>268</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>200</v>
+        <v>270</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>199</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>201</v>
+        <v>69</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>202</v>
+        <v>70</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>205</v>
+        <v>72</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>203</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>206</v>
+      <c r="A63" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>209</v>
+        <v>262</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>208</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>210</v>
+        <v>263</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>212</v>
+        <v>265</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>217</v>
+        <v>266</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>211</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>214</v>
+        <v>27</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>215</v>
+        <v>28</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>216</v>
+        <v>29</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>213</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>70</v>
+      <c r="A66" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>71</v>
+        <v>280</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>260</v>
+        <v>62</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>261</v>
+        <v>64</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>263</v>
+        <v>65</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>262</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>264</v>
+        <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>266</v>
+        <v>64</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>267</v>
+        <v>67</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>265</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>268</v>
+        <v>73</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>269</v>
+        <v>74</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>271</v>
+        <v>75</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>270</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{81FA332A-8EF1-4549-A3E8-9DC47654C3CA}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{75605A2A-2A43-D74F-99C7-EE6AE9B1387A}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{DB61C639-19F1-AB43-B8C0-AC6D20C4E12B}"/>
-    <hyperlink ref="D9" r:id="rId4" xr:uid="{7B6AA6D1-BC4B-2F4B-B8CC-B2273F527AED}"/>
-    <hyperlink ref="D10" r:id="rId5" xr:uid="{A85D9E62-8269-804F-80E7-53A9EB46BCB6}"/>
-    <hyperlink ref="D11" r:id="rId6" xr:uid="{187E11BF-B774-154E-B958-04088916D203}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{3134FC51-1C7C-6A41-94C1-26AA43037DF5}"/>
-    <hyperlink ref="D17" r:id="rId8" xr:uid="{3E1F2737-CB99-404C-A64B-A178B257FADC}"/>
-    <hyperlink ref="D19" r:id="rId9" xr:uid="{2C93FFDF-6D02-FB43-96B6-BE8CE0C6701B}"/>
-    <hyperlink ref="D18" r:id="rId10" xr:uid="{6EC04383-2256-914C-9AAC-57B183F659B4}"/>
-    <hyperlink ref="D54" r:id="rId11" xr:uid="{A21A88D2-6579-BE44-96A1-664F64FE55D7}"/>
-    <hyperlink ref="D20" r:id="rId12" xr:uid="{B417A120-DBCF-B141-9F65-88FABAF54B62}"/>
-    <hyperlink ref="D21" r:id="rId13" xr:uid="{20CE5E3D-C792-BF44-AA99-EEDC8CA11CD4}"/>
-    <hyperlink ref="D22" r:id="rId14" xr:uid="{CE5AA9F6-D3B2-444D-90F6-C463623EC47C}"/>
-    <hyperlink ref="D23" r:id="rId15" xr:uid="{676BCF16-5E47-7F43-B129-6C0ECAB8A1FD}"/>
-    <hyperlink ref="D24" r:id="rId16" xr:uid="{8BB9FA7E-5074-884F-BF96-701AE7B0C209}"/>
-    <hyperlink ref="D25" r:id="rId17" xr:uid="{D2A0C53C-9515-D04F-8A69-1FEAB98A084E}"/>
-    <hyperlink ref="D26" r:id="rId18" xr:uid="{EC78446D-D8C2-7D41-A868-52C097CD1104}"/>
-    <hyperlink ref="D66" r:id="rId19" xr:uid="{479A7FA6-FA6F-144D-B251-478FF39988F3}"/>
-    <hyperlink ref="D27" r:id="rId20" xr:uid="{6CB87E9C-0C57-7A4B-B3F8-29E4D2759EFB}"/>
-    <hyperlink ref="D29" r:id="rId21" xr:uid="{A89C030A-4C2A-0343-AA01-4C2B69454CBB}"/>
-    <hyperlink ref="D30" r:id="rId22" xr:uid="{F6A54C3A-1A60-0342-93B6-EFA09E232994}"/>
-    <hyperlink ref="D31" r:id="rId23" xr:uid="{AC58C7F5-E104-7A48-886C-8C26A9CADBDF}"/>
-    <hyperlink ref="D32" r:id="rId24" xr:uid="{9D679823-129A-4148-A25B-7BF002095F37}"/>
-    <hyperlink ref="D33" r:id="rId25" xr:uid="{BA9F6EFD-64FA-CB4D-9B45-3A55A614489B}"/>
-    <hyperlink ref="D34" r:id="rId26" xr:uid="{226288BA-73B4-194E-9BB1-05A9F762705E}"/>
-    <hyperlink ref="D35" r:id="rId27" xr:uid="{D3FCEC1C-8F22-B74D-B903-2907ECB753D2}"/>
-    <hyperlink ref="D36" r:id="rId28" xr:uid="{A82F7E7E-A704-EF42-8EFF-159283ACA9DE}"/>
-    <hyperlink ref="D28" r:id="rId29" xr:uid="{F2780EFF-1D3D-BC48-834D-EFF435AA2080}"/>
-    <hyperlink ref="D37" r:id="rId30" xr:uid="{77D35629-8CFB-3E4B-9BAB-EA727908ABFF}"/>
-    <hyperlink ref="D38" r:id="rId31" xr:uid="{7180229E-6E0F-024F-8A1A-D786EC0B4811}"/>
-    <hyperlink ref="D39" r:id="rId32" xr:uid="{1D5C85DA-EB65-F846-A4AB-F7AC5DD5A76B}"/>
-    <hyperlink ref="D40" r:id="rId33" xr:uid="{B35CA0CC-4481-DD46-9344-268C99D4811B}"/>
-    <hyperlink ref="D44" r:id="rId34" xr:uid="{186BA128-19D3-8747-ADA1-C2720A494347}"/>
-    <hyperlink ref="D41" r:id="rId35" xr:uid="{EEBDC5E5-F886-0148-8E36-809E5A377EE8}"/>
-    <hyperlink ref="D42" r:id="rId36" xr:uid="{4CBA85FB-C791-8E43-89A7-1196D9BD06F1}"/>
-    <hyperlink ref="D43" r:id="rId37" xr:uid="{9005E893-8AAF-BA40-80EE-5064E3E3F0B1}"/>
-    <hyperlink ref="D45" r:id="rId38" xr:uid="{1238868C-3272-D740-8313-083B91E2FE77}"/>
-    <hyperlink ref="D46" r:id="rId39" xr:uid="{AA85D42F-BC4F-8146-81DB-03775B9CB360}"/>
-    <hyperlink ref="D47" r:id="rId40" xr:uid="{B8F5A6E1-8C02-9D46-8B76-37A0B34E9C8A}"/>
-    <hyperlink ref="D48" r:id="rId41" xr:uid="{7A9E911C-89BC-3B48-9E80-AE85FAAEA921}"/>
-    <hyperlink ref="D49" r:id="rId42" xr:uid="{FE0D87B9-902B-0A43-8B5C-F222B9FA1123}"/>
-    <hyperlink ref="D52" r:id="rId43" xr:uid="{1C286A9C-9A1F-E340-B5F9-B71A344DCFCC}"/>
-    <hyperlink ref="D53" r:id="rId44" xr:uid="{F8DB7FFF-AE80-F946-9948-CB644CDE83DB}"/>
-    <hyperlink ref="D50" r:id="rId45" xr:uid="{C31CF6DF-6801-3849-8E9A-50B9DB84D3A8}"/>
-    <hyperlink ref="D56" r:id="rId46" xr:uid="{021A3E40-1E44-1246-B394-683AE93DEBD8}"/>
-    <hyperlink ref="D57" r:id="rId47" xr:uid="{49BE09A2-01E3-C845-8B0D-7BEED56B0438}"/>
-    <hyperlink ref="D58" r:id="rId48" xr:uid="{2917C5C7-925E-6543-9F69-9D2FB89136F6}"/>
-    <hyperlink ref="D59" r:id="rId49" xr:uid="{D51E8A99-A855-A34D-ACDB-796DBF858E96}"/>
-    <hyperlink ref="D60" r:id="rId50" xr:uid="{63CA1618-1153-1A44-B560-FE819F2D56B7}"/>
-    <hyperlink ref="D61" r:id="rId51" xr:uid="{F4F03AF2-517D-4546-B550-E759A049CBC8}"/>
-    <hyperlink ref="D62" r:id="rId52" xr:uid="{A7D40954-4185-E84A-8C06-0F963AF40A64}"/>
-    <hyperlink ref="D63" r:id="rId53" xr:uid="{06143F55-4844-FB41-A6C5-15C7C0866752}"/>
-    <hyperlink ref="D64" r:id="rId54" xr:uid="{52C6A777-CAE1-B744-A3D6-6DDB27155772}"/>
-    <hyperlink ref="D65" r:id="rId55" xr:uid="{E51A6A59-561F-EA4E-A3C0-59D6DEC4E061}"/>
-    <hyperlink ref="D4" r:id="rId56" xr:uid="{44E395AA-7E54-D94E-85D9-6AAF326C142E}"/>
-    <hyperlink ref="D2" r:id="rId57" xr:uid="{AE1502FC-4861-0F43-8DE9-AF0402F1CF4D}"/>
-    <hyperlink ref="D5" r:id="rId58" xr:uid="{D931EC70-0A44-0F4C-8516-0C28E03B6101}"/>
-    <hyperlink ref="D12" r:id="rId59" xr:uid="{11316C23-A969-994E-985D-9D9F10D662B7}"/>
-    <hyperlink ref="D8" r:id="rId60" xr:uid="{71752224-60BB-E94B-A0CA-5BA804917649}"/>
-    <hyperlink ref="D14" r:id="rId61" xr:uid="{FDE2143A-7188-4F44-9774-E4EBA09564E5}"/>
-    <hyperlink ref="D16" r:id="rId62" xr:uid="{B6173CF0-8D3D-DE43-9C97-9103716C2930}"/>
-    <hyperlink ref="D15" r:id="rId63" xr:uid="{B5EFB8B9-E050-004A-BD65-2E684919A50E}"/>
-    <hyperlink ref="D51" r:id="rId64" xr:uid="{4DC3E40C-8B70-FA40-A3E4-25E1734BDAFB}"/>
-    <hyperlink ref="D55" r:id="rId65" xr:uid="{4D2C1141-9A97-9644-8E45-216BD13BFF89}"/>
-    <hyperlink ref="D67" r:id="rId66" xr:uid="{E20CBFFF-001E-C84C-BB28-2ADC45304E0D}"/>
-    <hyperlink ref="D68" r:id="rId67" xr:uid="{1846E8D2-0B76-704F-860F-4E3927F991B5}"/>
-    <hyperlink ref="D69" r:id="rId68" xr:uid="{0946BD1E-9AAC-2146-969D-141285FDF27E}"/>
+    <hyperlink ref="D50" r:id="rId1" xr:uid="{81FA332A-8EF1-4549-A3E8-9DC47654C3CA}"/>
+    <hyperlink ref="D47" r:id="rId2" xr:uid="{75605A2A-2A43-D74F-99C7-EE6AE9B1387A}"/>
+    <hyperlink ref="D51" r:id="rId3" xr:uid="{DB61C639-19F1-AB43-B8C0-AC6D20C4E12B}"/>
+    <hyperlink ref="D55" r:id="rId4" xr:uid="{7B6AA6D1-BC4B-2F4B-B8CC-B2273F527AED}"/>
+    <hyperlink ref="D56" r:id="rId5" xr:uid="{A85D9E62-8269-804F-80E7-53A9EB46BCB6}"/>
+    <hyperlink ref="D57" r:id="rId6" xr:uid="{187E11BF-B774-154E-B958-04088916D203}"/>
+    <hyperlink ref="D53" r:id="rId7" xr:uid="{3134FC51-1C7C-6A41-94C1-26AA43037DF5}"/>
+    <hyperlink ref="D65" r:id="rId8" xr:uid="{3E1F2737-CB99-404C-A64B-A178B257FADC}"/>
+    <hyperlink ref="D73" r:id="rId9" xr:uid="{2C93FFDF-6D02-FB43-96B6-BE8CE0C6701B}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{6EC04383-2256-914C-9AAC-57B183F659B4}"/>
+    <hyperlink ref="D32" r:id="rId11" xr:uid="{A21A88D2-6579-BE44-96A1-664F64FE55D7}"/>
+    <hyperlink ref="D4" r:id="rId12" xr:uid="{B417A120-DBCF-B141-9F65-88FABAF54B62}"/>
+    <hyperlink ref="D12" r:id="rId13" xr:uid="{20CE5E3D-C792-BF44-AA99-EEDC8CA11CD4}"/>
+    <hyperlink ref="D13" r:id="rId14" xr:uid="{CE5AA9F6-D3B2-444D-90F6-C463623EC47C}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{676BCF16-5E47-7F43-B129-6C0ECAB8A1FD}"/>
+    <hyperlink ref="D66" r:id="rId16" xr:uid="{8BB9FA7E-5074-884F-BF96-701AE7B0C209}"/>
+    <hyperlink ref="D67" r:id="rId17" xr:uid="{D2A0C53C-9515-D04F-8A69-1FEAB98A084E}"/>
+    <hyperlink ref="D68" r:id="rId18" xr:uid="{EC78446D-D8C2-7D41-A868-52C097CD1104}"/>
+    <hyperlink ref="D62" r:id="rId19" xr:uid="{479A7FA6-FA6F-144D-B251-478FF39988F3}"/>
+    <hyperlink ref="D69" r:id="rId20" xr:uid="{6CB87E9C-0C57-7A4B-B3F8-29E4D2759EFB}"/>
+    <hyperlink ref="D70" r:id="rId21" xr:uid="{A89C030A-4C2A-0343-AA01-4C2B69454CBB}"/>
+    <hyperlink ref="D71" r:id="rId22" xr:uid="{F6A54C3A-1A60-0342-93B6-EFA09E232994}"/>
+    <hyperlink ref="D72" r:id="rId23" xr:uid="{AC58C7F5-E104-7A48-886C-8C26A9CADBDF}"/>
+    <hyperlink ref="D3" r:id="rId24" xr:uid="{9D679823-129A-4148-A25B-7BF002095F37}"/>
+    <hyperlink ref="D5" r:id="rId25" xr:uid="{BA9F6EFD-64FA-CB4D-9B45-3A55A614489B}"/>
+    <hyperlink ref="D6" r:id="rId26" xr:uid="{226288BA-73B4-194E-9BB1-05A9F762705E}"/>
+    <hyperlink ref="D8" r:id="rId27" xr:uid="{D3FCEC1C-8F22-B74D-B903-2907ECB753D2}"/>
+    <hyperlink ref="D9" r:id="rId28" xr:uid="{A82F7E7E-A704-EF42-8EFF-159283ACA9DE}"/>
+    <hyperlink ref="D10" r:id="rId29" xr:uid="{F2780EFF-1D3D-BC48-834D-EFF435AA2080}"/>
+    <hyperlink ref="D15" r:id="rId30" xr:uid="{77D35629-8CFB-3E4B-9BAB-EA727908ABFF}"/>
+    <hyperlink ref="D16" r:id="rId31" xr:uid="{7180229E-6E0F-024F-8A1A-D786EC0B4811}"/>
+    <hyperlink ref="D17" r:id="rId32" xr:uid="{1D5C85DA-EB65-F846-A4AB-F7AC5DD5A76B}"/>
+    <hyperlink ref="D18" r:id="rId33" xr:uid="{B35CA0CC-4481-DD46-9344-268C99D4811B}"/>
+    <hyperlink ref="D22" r:id="rId34" xr:uid="{186BA128-19D3-8747-ADA1-C2720A494347}"/>
+    <hyperlink ref="D19" r:id="rId35" xr:uid="{EEBDC5E5-F886-0148-8E36-809E5A377EE8}"/>
+    <hyperlink ref="D20" r:id="rId36" xr:uid="{4CBA85FB-C791-8E43-89A7-1196D9BD06F1}"/>
+    <hyperlink ref="D21" r:id="rId37" xr:uid="{9005E893-8AAF-BA40-80EE-5064E3E3F0B1}"/>
+    <hyperlink ref="D23" r:id="rId38" xr:uid="{1238868C-3272-D740-8313-083B91E2FE77}"/>
+    <hyperlink ref="D24" r:id="rId39" xr:uid="{AA85D42F-BC4F-8146-81DB-03775B9CB360}"/>
+    <hyperlink ref="D25" r:id="rId40" xr:uid="{B8F5A6E1-8C02-9D46-8B76-37A0B34E9C8A}"/>
+    <hyperlink ref="D26" r:id="rId41" xr:uid="{7A9E911C-89BC-3B48-9E80-AE85FAAEA921}"/>
+    <hyperlink ref="D27" r:id="rId42" xr:uid="{FE0D87B9-902B-0A43-8B5C-F222B9FA1123}"/>
+    <hyperlink ref="D30" r:id="rId43" xr:uid="{1C286A9C-9A1F-E340-B5F9-B71A344DCFCC}"/>
+    <hyperlink ref="D31" r:id="rId44" xr:uid="{F8DB7FFF-AE80-F946-9948-CB644CDE83DB}"/>
+    <hyperlink ref="D28" r:id="rId45" xr:uid="{C31CF6DF-6801-3849-8E9A-50B9DB84D3A8}"/>
+    <hyperlink ref="D34" r:id="rId46" xr:uid="{021A3E40-1E44-1246-B394-683AE93DEBD8}"/>
+    <hyperlink ref="D35" r:id="rId47" xr:uid="{49BE09A2-01E3-C845-8B0D-7BEED56B0438}"/>
+    <hyperlink ref="D36" r:id="rId48" xr:uid="{2917C5C7-925E-6543-9F69-9D2FB89136F6}"/>
+    <hyperlink ref="D38" r:id="rId49" xr:uid="{D51E8A99-A855-A34D-ACDB-796DBF858E96}"/>
+    <hyperlink ref="D40" r:id="rId50" xr:uid="{63CA1618-1153-1A44-B560-FE819F2D56B7}"/>
+    <hyperlink ref="D41" r:id="rId51" xr:uid="{F4F03AF2-517D-4546-B550-E759A049CBC8}"/>
+    <hyperlink ref="D42" r:id="rId52" xr:uid="{A7D40954-4185-E84A-8C06-0F963AF40A64}"/>
+    <hyperlink ref="D43" r:id="rId53" xr:uid="{06143F55-4844-FB41-A6C5-15C7C0866752}"/>
+    <hyperlink ref="D44" r:id="rId54" xr:uid="{52C6A777-CAE1-B744-A3D6-6DDB27155772}"/>
+    <hyperlink ref="D45" r:id="rId55" xr:uid="{E51A6A59-561F-EA4E-A3C0-59D6DEC4E061}"/>
+    <hyperlink ref="D48" r:id="rId56" xr:uid="{44E395AA-7E54-D94E-85D9-6AAF326C142E}"/>
+    <hyperlink ref="D46" r:id="rId57" xr:uid="{AE1502FC-4861-0F43-8DE9-AF0402F1CF4D}"/>
+    <hyperlink ref="D49" r:id="rId58" xr:uid="{D931EC70-0A44-0F4C-8516-0C28E03B6101}"/>
+    <hyperlink ref="D58" r:id="rId59" xr:uid="{11316C23-A969-994E-985D-9D9F10D662B7}"/>
+    <hyperlink ref="D52" r:id="rId60" xr:uid="{71752224-60BB-E94B-A0CA-5BA804917649}"/>
+    <hyperlink ref="D54" r:id="rId61" xr:uid="{FDE2143A-7188-4F44-9774-E4EBA09564E5}"/>
+    <hyperlink ref="D60" r:id="rId62" xr:uid="{B6173CF0-8D3D-DE43-9C97-9103716C2930}"/>
+    <hyperlink ref="D59" r:id="rId63" xr:uid="{B5EFB8B9-E050-004A-BD65-2E684919A50E}"/>
+    <hyperlink ref="D29" r:id="rId64" xr:uid="{4DC3E40C-8B70-FA40-A3E4-25E1734BDAFB}"/>
+    <hyperlink ref="D33" r:id="rId65" xr:uid="{4D2C1141-9A97-9644-8E45-216BD13BFF89}"/>
+    <hyperlink ref="D63" r:id="rId66" xr:uid="{E20CBFFF-001E-C84C-BB28-2ADC45304E0D}"/>
+    <hyperlink ref="D64" r:id="rId67" xr:uid="{1846E8D2-0B76-704F-860F-4E3927F991B5}"/>
+    <hyperlink ref="D61" r:id="rId68" xr:uid="{0946BD1E-9AAC-2146-969D-141285FDF27E}"/>
+    <hyperlink ref="D2" r:id="rId69" xr:uid="{79A1D728-11A4-5C4F-B192-B8D7E8216536}"/>
+    <hyperlink ref="D11" r:id="rId70" xr:uid="{E34D0B28-1D2E-6B46-BBB3-F692FBF88F42}"/>
+    <hyperlink ref="D74" r:id="rId71" xr:uid="{0ADDEC52-FE91-1546-BFE1-6672CF0D9CD1}"/>
+    <hyperlink ref="D39" r:id="rId72" xr:uid="{30F1C9F0-4183-2F46-AD6F-8EC7E11BEDCB}"/>
+    <hyperlink ref="D75" r:id="rId73" xr:uid="{31006679-DE45-3840-863E-012D968FBB16}"/>
+    <hyperlink ref="D76" r:id="rId74" xr:uid="{55F7F737-441B-C34B-BD9B-EC1D733EF2F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>